<commit_message>
Actualizacion del espacio de reporte
</commit_message>
<xml_diff>
--- a/Organización/Procesos/Ciclo de vida IWM/3. Ejecución/3.3 Pruebas internas/PTTL_casos_de_prueba.xlsx
+++ b/Organización/Procesos/Ciclo de vida IWM/3. Ejecución/3.3 Pruebas internas/PTTL_casos_de_prueba.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Casos De Uso</t>
   </si>
@@ -39,28 +39,22 @@
     <t>Caso de Prueba</t>
   </si>
   <si>
-    <t>Reporte de revision</t>
-  </si>
-  <si>
     <t>Nombre del proyecto:</t>
   </si>
   <si>
-    <t>Tipo de revision:</t>
-  </si>
-  <si>
     <t>Fecha:</t>
   </si>
   <si>
     <t>Elaborado por (autor del documento):</t>
   </si>
   <si>
-    <t>Inspector(es):</t>
-  </si>
-  <si>
     <t>Tiempo de realizacion:</t>
   </si>
   <si>
     <t>Requerimientos:</t>
+  </si>
+  <si>
+    <t>Reporte</t>
   </si>
 </sst>
 </file>
@@ -249,13 +243,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Celda de comprobación" xfId="1" builtinId="23"/>
@@ -561,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H34"/>
+  <dimension ref="B2:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:D6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,85 +572,87 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-    </row>
-    <row r="10" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="8"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="8"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="4"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" s="1"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="4"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
@@ -810,40 +806,22 @@
       <c r="F31" s="2"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="4"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="4"/>
-    </row>
-    <row r="34" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="5"/>
+    <row r="32" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
+  <mergeCells count="6">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>